<commit_message>
update font config and move preprocessor into a file
</commit_message>
<xml_diff>
--- a/configuration/fontExperiment.xlsx
+++ b/configuration/fontExperiment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denispelli/Dropbox/Font project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peilingjiang/Documents/github/EasyEyes/crowding/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5A6903-3563-C342-BF12-36166B7618C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD698D47-9ACD-0C47-B30A-B76477B9312D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="16500" windowHeight="14740" xr2:uid="{F69C2BA8-47DB-F84B-AF65-B4108097FF78}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="27820" windowHeight="17500" xr2:uid="{F69C2BA8-47DB-F84B-AF65-B4108097FF78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
   <si>
     <t>conditionName</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>aboutDateModified</t>
+  </si>
+  <si>
+    <t>wirelessKeyboardNeededYes</t>
   </si>
 </sst>
 </file>
@@ -576,14 +579,16 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="1"/>
@@ -616,6 +621,15 @@
       <c r="B1" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="C1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
@@ -624,6 +638,15 @@
       <c r="B2" s="8">
         <v>44409</v>
       </c>
+      <c r="C2" s="8">
+        <v>44409</v>
+      </c>
+      <c r="D2" s="8">
+        <v>44409</v>
+      </c>
+      <c r="E2" s="8">
+        <v>44409</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -632,6 +655,15 @@
       <c r="B3" s="8">
         <v>44423</v>
       </c>
+      <c r="C3" s="8">
+        <v>44423</v>
+      </c>
+      <c r="D3" s="8">
+        <v>44423</v>
+      </c>
+      <c r="E3" s="8">
+        <v>44423</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -640,6 +672,15 @@
       <c r="B4" s="8" t="s">
         <v>47</v>
       </c>
+      <c r="C4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -648,6 +689,15 @@
       <c r="B5" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="C5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1165,7 +1215,21 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37"/>
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E5">
@@ -1173,6 +1237,9 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{1134B44E-E201-AF4A-8341-A238506DFAC9}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{BE4C07E9-94B9-5349-B8A1-F4204DFE0077}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{D44FADA4-62F1-7E4E-ABEC-2ADA866179AD}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{7C1C45C6-E1A5-CF44-8D2C-8B0E0629653D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>